<commit_message>
General config and HU-CP001
General: Adding timestamp to execution evidences folder, adding json utils, adding testutils and creating custom reporter. HU1-CP001: Validating ux
</commit_message>
<xml_diff>
--- a/test_info/data/HU1-001/objects.xlsx
+++ b/test_info/data/HU1-001/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan_piedrahita\Documents\jp\bvc\tests\A2censoTest\test_info\data\HU1-001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94597305-FFD3-4F79-AEF0-5711A62CB9FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5A80A8-D2AE-41CF-8796-7C09E28C404B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{58DB2863-25CE-48F2-AA27-D6192448486C}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{58DB2863-25CE-48F2-AA27-D6192448486C}"/>
   </bookViews>
   <sheets>
     <sheet name="menu" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -64,9 +64,6 @@
     <t>menu</t>
   </si>
   <si>
-    <t>visibility</t>
-  </si>
-  <si>
     <t>logo</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>navbar</t>
+  </si>
+  <si>
+    <t>visible</t>
   </si>
 </sst>
 </file>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83524DA6-37D5-46FC-ACE2-F9959D21CE3A}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,77 +511,77 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -590,7 +590,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -604,7 +604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE08B081-540D-41FE-A0DF-5A4050755188}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -629,68 +629,70 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -703,7 +705,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -717,7 +719,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>